<commit_message>
feat: Connection in DB
</commit_message>
<xml_diff>
--- a/TestProject1/DDT/Rotina_1801.xlsx
+++ b/TestProject1/DDT/Rotina_1801.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="DADOS" sheetId="1" r:id="rId1"/>
@@ -61,9 +61,6 @@
     <t>200016</t>
   </si>
   <si>
-    <t>test</t>
-  </si>
-  <si>
     <t>Dinheiro</t>
   </si>
   <si>
@@ -80,6 +77,9 @@
   </si>
   <si>
     <t>Outras</t>
+  </si>
+  <si>
+    <t>test123</t>
   </si>
 </sst>
 </file>
@@ -434,17 +434,17 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.21875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -479,30 +479,30 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>14</v>

</xml_diff>